<commit_message>
Borrado callao de lima
</commit_message>
<xml_diff>
--- a/central_table-LIMA.xlsx
+++ b/central_table-LIMA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Personal\Desktop\Archivos-varios\lr\investigaciones\dengue-tesst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Personal\Desktop\cosas personales jl\codigo\scraping-beautiful-dengue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4732E1-8B47-45FB-9185-F36B10F1EB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02161C5C-7BFB-43A1-B44E-65E7E1582B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2885E2BF-BFA2-49F0-A74C-B4B583AB3860}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Distrito</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>BREÑA</t>
-  </si>
-  <si>
-    <t>CALLAO</t>
   </si>
   <si>
     <t>CARABAYLLO</t>
@@ -558,17 +555,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF11FA8-D4E2-46BC-97F0-3B678C839BA4}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -625,7 +622,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -633,7 +630,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -641,7 +638,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -649,7 +646,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
@@ -657,7 +654,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -665,7 +662,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
@@ -673,7 +670,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
@@ -681,7 +678,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -689,7 +686,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -697,7 +694,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>18</v>
@@ -705,7 +702,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>19</v>
@@ -713,7 +710,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
@@ -721,7 +718,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>21</v>
@@ -729,7 +726,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
@@ -737,7 +734,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
@@ -745,7 +742,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
@@ -753,7 +750,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
@@ -761,7 +758,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>26</v>
@@ -769,7 +766,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>27</v>
@@ -777,23 +774,23 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>29</v>
@@ -801,7 +798,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>30</v>
@@ -809,7 +806,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>31</v>
@@ -817,7 +814,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>32</v>
@@ -825,7 +822,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>33</v>
@@ -833,7 +830,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>34</v>
@@ -841,7 +838,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>35</v>
@@ -849,7 +846,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>36</v>
@@ -857,7 +854,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>37</v>
@@ -865,7 +862,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>38</v>
@@ -873,7 +870,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>39</v>
@@ -881,7 +878,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>40</v>
@@ -889,7 +886,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>41</v>
@@ -897,7 +894,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>42</v>
@@ -905,7 +902,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>43</v>
@@ -913,7 +910,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>44</v>
@@ -921,7 +918,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>45</v>
@@ -929,7 +926,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>46</v>
@@ -937,7 +934,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>47</v>
@@ -945,7 +942,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>48</v>
@@ -953,7 +950,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>49</v>
@@ -961,7 +958,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>50</v>
@@ -969,18 +966,10 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
-        <v>28</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>